<commit_message>
agregando sistema de puntaje
</commit_message>
<xml_diff>
--- a/practica5/mapa.xlsx
+++ b/practica5/mapa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Documents\Curso Informatica 2\Laboratorio\practica5\practica5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A4D0C5-586E-4A3B-A3A6-D060E7388D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AF6C9E2-8F15-4FA2-9722-D74A0E3AA2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18F12D3D-DD15-4D66-A88C-D1D52780EDCF}"/>
   </bookViews>
@@ -71,37 +71,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -535,7 +505,7 @@
   <dimension ref="A1:BV49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="AY2" sqref="AY2:BV22"/>
+      <selection activeCell="BP20" sqref="BP20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1196,7 +1166,7 @@
         <v>2</v>
       </c>
       <c r="BC4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BD4">
         <v>2</v>
@@ -1235,7 +1205,7 @@
         <v>2</v>
       </c>
       <c r="BP4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BQ4">
         <v>1</v>
@@ -4636,7 +4606,7 @@
         <v>2</v>
       </c>
       <c r="BC20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BD20">
         <v>2</v>
@@ -4675,7 +4645,7 @@
         <v>2</v>
       </c>
       <c r="BP20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BQ20">
         <v>1</v>
@@ -6964,41 +6934,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="P8:T12 B3:T7 B8:F12 B17:T24 G11:H12 I11:O11 N12:O12 G8:O10 H13 B14:H16 N13:T16 I12:M16">
-    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE17:AI21 Z3:AD21 AE3:AI7 AN3:AU21 AH8:AI9 AH10:AH16 AI15:AI16 AE8:AG16 AJ9 AK3:AM9 AJ15:AM21 AI10:AM14">
-    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3">
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM32:AQ36 Y27:AQ31 Y32:AC36 Y41:AQ48 AD35:AE36 AF35:AL35 AK36:AL36 AD32:AL34 AE37 Y38:AE40 AK37:AQ40 AF36:AJ40">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y37">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>